<commit_message>
finalizing revC schematic and board
</commit_message>
<xml_diff>
--- a/kicad/BOM.xlsx
+++ b/kicad/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38DD6AC-E2A1-4B9A-BCE5-EABF07A1E8D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265377DD-094E-4CE9-ADDA-D2C1DF4F76A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="174">
   <si>
     <t>Ref</t>
   </si>
@@ -472,9 +472,6 @@
     <t>Enclosure</t>
   </si>
   <si>
-    <t>1455L801</t>
-  </si>
-  <si>
     <t>GPS Module</t>
   </si>
   <si>
@@ -520,13 +517,31 @@
     <t>SMD 1207</t>
   </si>
   <si>
-    <t>L2, L3</t>
-  </si>
-  <si>
-    <t>C3, C32</t>
-  </si>
-  <si>
-    <t>C6, C7, C9, C10, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C26, C33</t>
+    <t>DMP3099L</t>
+  </si>
+  <si>
+    <t>DMP3099L-13</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3, C32, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6, C7, C9, C10, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C26, C33, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2, L3, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1, </t>
+  </si>
+  <si>
+    <t>1455K1201</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,11 +1436,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F1" s="7">
-        <f>SUM(G3:G70)</f>
-        <v>90.691999999999979</v>
+        <f>SUM(G3:G72)</f>
+        <v>88.021999999999991</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1477,7 +1492,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1486,7 +1501,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
         <v>107</v>
@@ -1495,7 +1510,7 @@
         <v>0.31</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G49" si="0">F4*B4</f>
+        <f t="shared" ref="G4:G51" si="0">F4*B4</f>
         <v>0.62</v>
       </c>
     </row>
@@ -1549,7 +1564,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B7">
         <v>17</v>
@@ -1582,7 +1597,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
@@ -1606,7 +1621,7 @@
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" t="s">
         <v>107</v>
@@ -1789,209 +1804,205 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.76</v>
-      </c>
+      <c r="C17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="8"/>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F18" s="3">
-        <v>0.19</v>
+        <v>0.76</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
-        <v>0.19</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
+      </c>
+      <c r="E19" t="s">
+        <v>113</v>
       </c>
       <c r="F19" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.19</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F20" s="3">
-        <v>2.61</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>2.61</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="4">
-        <v>734152980</v>
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F21" s="3">
-        <v>6.18</v>
+        <v>2.61</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="0"/>
-        <v>12.36</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" t="s">
-        <v>120</v>
+        <v>35</v>
+      </c>
+      <c r="D22" s="4">
+        <v>734152980</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="F22" s="3">
-        <v>0.86</v>
+        <v>6.18</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="0"/>
-        <v>0.86</v>
+        <v>12.36</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>111</v>
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>120</v>
       </c>
       <c r="F23" s="3">
-        <v>3.05</v>
+        <v>0.86</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" si="0"/>
-        <v>3.05</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>121</v>
+        <v>111</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3.05</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.05</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="E25" s="8"/>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1999,112 +2010,105 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>164</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F27" s="3">
-        <v>0.33</v>
+        <v>0.16</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
-        <v>0.66</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>46</v>
+      <c r="C28" t="s">
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="F28" s="3">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="F29" s="3">
-        <v>5.7000000000000002E-2</v>
+        <v>0.33</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>
-        <v>0.34200000000000003</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>94</v>
@@ -2119,40 +2123,40 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="3">
-        <v>0.1</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B32">
-        <v>5</v>
-      </c>
-      <c r="C32" s="4">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>94</v>
@@ -2162,21 +2166,21 @@
       </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" s="4">
-        <v>470</v>
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>94</v>
@@ -2186,21 +2190,21 @@
       </c>
       <c r="G33" s="3">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="C34" s="4">
+        <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>94</v>
@@ -2210,21 +2214,21 @@
       </c>
       <c r="G34" s="3">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>58</v>
+      <c r="C35" s="4">
+        <v>470</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>94</v>
@@ -2239,16 +2243,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" t="s">
-        <v>158</v>
+      <c r="C36" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D36" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>94</v>
@@ -2263,75 +2267,89 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="F37" s="3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E38" s="8"/>
+        <v>157</v>
+      </c>
+      <c r="D38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.1</v>
+      </c>
       <c r="G38" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.2</v>
+      </c>
       <c r="G39" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="G40" s="3">
         <f t="shared" si="0"/>
@@ -2340,310 +2358,346 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.9</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
       <c r="G41" s="3">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F42" s="3">
-        <v>4.08</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
       <c r="G42" s="3">
         <f t="shared" si="0"/>
-        <v>4.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F43" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="G43" s="3">
         <f t="shared" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="E44" t="s">
+        <v>134</v>
       </c>
       <c r="F44" s="3">
-        <v>0.57999999999999996</v>
+        <v>4.08</v>
       </c>
       <c r="G44" s="3">
         <f t="shared" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F45" s="3">
-        <v>2.81</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G45" s="3">
         <f t="shared" si="0"/>
-        <v>5.62</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" t="s">
-        <v>140</v>
+        <v>75</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="F46" s="3">
-        <v>1.99</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G46" s="3">
         <f t="shared" si="0"/>
-        <v>1.99</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="F47" s="3">
-        <v>0.44</v>
+        <v>2.81</v>
       </c>
       <c r="G47" s="3">
         <f t="shared" si="0"/>
-        <v>0.44</v>
+        <v>5.62</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+      <c r="E48" t="s">
+        <v>140</v>
       </c>
       <c r="F48" s="3">
-        <v>0.33</v>
+        <v>1.99</v>
       </c>
       <c r="G48" s="3">
         <f t="shared" si="0"/>
-        <v>0.33</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" t="s">
-        <v>144</v>
+        <v>81</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="F49" s="3">
-        <v>10</v>
+        <v>0.44</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D51" t="s">
-        <v>147</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>121</v>
+        <v>143</v>
+      </c>
+      <c r="E51" t="s">
+        <v>144</v>
       </c>
       <c r="F51" s="3">
-        <v>1.33</v>
+        <v>10</v>
       </c>
       <c r="G51" s="3">
-        <f t="shared" ref="G51:G53" si="1">B51*F51</f>
-        <v>1.33</v>
-      </c>
-      <c r="I51" t="s">
-        <v>148</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>149</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" t="s">
-        <v>150</v>
-      </c>
-      <c r="E52" t="s">
-        <v>121</v>
-      </c>
-      <c r="F52" s="3">
-        <v>21</v>
-      </c>
-      <c r="G52" s="3">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
+      <c r="A52" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" ref="G53:G55" si="1">B53*F53</f>
+        <v>1.33</v>
+      </c>
+      <c r="I53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" s="3">
+        <v>18</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
         <v>151</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D55" t="s">
         <v>152</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E55" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F53" s="3">
+      <c r="F55" s="3">
         <v>12</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G55" s="3">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D38:E40"/>
-    <mergeCell ref="A50:G50"/>
+  <mergeCells count="4">
+    <mergeCell ref="D40:E42"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
updated BOM with new components
</commit_message>
<xml_diff>
--- a/kicad/BOM.xlsx
+++ b/kicad/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\GitHub\Simple-GPSDO\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265377DD-094E-4CE9-ADDA-D2C1DF4F76A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8DCC89-3E33-45D0-ACC6-387A5E6BD387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="184">
   <si>
     <t>Ref</t>
   </si>
@@ -542,6 +542,36 @@
   </si>
   <si>
     <t>1455K1201</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>68R</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>2R</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Warnings</t>
+  </si>
+  <si>
+    <t>SMD 0806</t>
+  </si>
+  <si>
+    <t>SMD 0807</t>
+  </si>
+  <si>
+    <t>CRCW080568R0FKEA</t>
+  </si>
+  <si>
+    <t>CRCW08052R00FKEA</t>
   </si>
 </sst>
 </file>
@@ -551,7 +581,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,6 +728,12 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1045,7 +1081,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1061,6 +1097,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="17" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1108,7 +1147,36 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1418,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,18 +1500,20 @@
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E1" s="6" t="s">
         <v>154</v>
       </c>
       <c r="F1" s="7">
-        <f>SUM(G3:G72)</f>
-        <v>88.021999999999991</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <f>SUM(G3:G74)</f>
+        <v>88.22199999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,8 +1535,14 @@
       <c r="G2" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1489,8 +1565,12 @@
         <f>F3*B3</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" t="str">
+        <f>IF(AND(A3 &lt;&gt; "",D3 = ""), "⚠️No P/N","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -1510,11 +1590,15 @@
         <v>0.31</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G51" si="0">F4*B4</f>
+        <f t="shared" ref="G4:G53" si="0">F4*B4</f>
         <v>0.62</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I61" si="1">IF(AND(A4 &lt;&gt; "",D4 = ""), "⚠️No P/N","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1537,8 +1621,12 @@
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1561,8 +1649,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -1585,8 +1677,12 @@
         <f t="shared" si="0"/>
         <v>0.85000000000000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1609,8 +1705,12 @@
         <f t="shared" si="0"/>
         <v>0.98</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1633,8 +1733,12 @@
         <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1657,8 +1761,12 @@
         <f t="shared" si="0"/>
         <v>0.37</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1681,8 +1789,12 @@
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1705,8 +1817,12 @@
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1729,8 +1845,12 @@
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1753,8 +1873,12 @@
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1777,8 +1901,12 @@
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1801,8 +1929,12 @@
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -1820,8 +1952,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1844,8 +1980,12 @@
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1868,8 +2008,12 @@
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1892,8 +2036,12 @@
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1916,8 +2064,12 @@
         <f t="shared" si="0"/>
         <v>2.61</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1940,8 +2092,12 @@
         <f t="shared" si="0"/>
         <v>12.36</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1964,8 +2120,12 @@
         <f t="shared" si="0"/>
         <v>0.86</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1988,8 +2148,12 @@
         <f t="shared" si="0"/>
         <v>3.05</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1999,16 +2163,20 @@
       <c r="C25" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="10"/>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2018,14 +2186,20 @@
       <c r="C26" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2048,8 +2222,12 @@
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>171</v>
       </c>
@@ -2072,8 +2250,12 @@
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -2096,8 +2278,12 @@
         <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -2120,8 +2306,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -2144,8 +2334,12 @@
         <f t="shared" si="0"/>
         <v>0.34200000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2168,8 +2362,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2192,8 +2390,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -2216,8 +2418,12 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -2240,8 +2446,12 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -2264,8 +2474,12 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -2288,8 +2502,12 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -2312,393 +2530,555 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>60</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>61</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D41" t="s">
         <v>130</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F41" s="3">
         <v>0.2</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G41" s="3">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>62</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D42" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="G40" s="3">
+      <c r="E42" s="10"/>
+      <c r="G42" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="I42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="G41" s="3">
+      <c r="D43" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="G43" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="I43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>66</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="G42" s="3">
+      <c r="D44" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="G44" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>68</v>
       </c>
-      <c r="B43">
+      <c r="B45">
         <v>2</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>69</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F45" s="3">
         <v>0.9</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G45" s="3">
         <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="I45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
         <v>71</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>133</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E46" t="s">
         <v>134</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F46" s="3">
         <v>4.08</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G46" s="3">
         <f t="shared" si="0"/>
         <v>4.08</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>72</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>73</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F47" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G47" s="3">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>74</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
         <v>75</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F48" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G48" s="3">
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
-      </c>
-      <c r="C47" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" t="s">
-        <v>137</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F47" s="3">
-        <v>2.81</v>
-      </c>
-      <c r="G47" s="3">
-        <f t="shared" si="0"/>
-        <v>5.62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" t="s">
-        <v>139</v>
-      </c>
-      <c r="E48" t="s">
-        <v>140</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1.99</v>
-      </c>
-      <c r="G48" s="3">
-        <f t="shared" si="0"/>
-        <v>1.99</v>
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="F49" s="3">
-        <v>0.44</v>
+        <v>2.81</v>
       </c>
       <c r="G49" s="3">
         <f t="shared" si="0"/>
-        <v>0.44</v>
+        <v>5.62</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+      <c r="E50" t="s">
+        <v>140</v>
       </c>
       <c r="F50" s="3">
-        <v>0.33</v>
+        <v>1.99</v>
       </c>
       <c r="G50" s="3">
         <f t="shared" si="0"/>
-        <v>0.33</v>
+        <v>1.99</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
-      </c>
-      <c r="E51" t="s">
-        <v>144</v>
+        <v>81</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="F51" s="3">
-        <v>10</v>
+        <v>0.44</v>
       </c>
       <c r="G51" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.44</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
-        <v>147</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>121</v>
+        <v>143</v>
+      </c>
+      <c r="E53" t="s">
+        <v>144</v>
       </c>
       <c r="F53" s="3">
-        <v>1.33</v>
+        <v>10</v>
       </c>
       <c r="G53" s="3">
-        <f t="shared" ref="G53:G55" si="1">B53*F53</f>
-        <v>1.33</v>
-      </c>
-      <c r="I53" t="s">
-        <v>148</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>149</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D54" t="s">
-        <v>173</v>
-      </c>
-      <c r="E54" t="s">
-        <v>121</v>
-      </c>
-      <c r="F54" s="3">
-        <v>18</v>
-      </c>
-      <c r="G54" s="3">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
+      <c r="A54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" ref="G55:G57" si="2">B55*F55</f>
+        <v>1.33</v>
+      </c>
+      <c r="H55" t="s">
+        <v>148</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" t="s">
+        <v>121</v>
+      </c>
+      <c r="F56" s="3">
+        <v>18</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>150</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
         <v>151</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>152</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F57" s="3">
         <v>12</v>
       </c>
-      <c r="G55" s="3">
-        <f t="shared" si="1"/>
+      <c r="G57" s="3">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I61" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I62" t="str">
+        <f t="shared" ref="I4:I62" si="3">IF(AND(A62 &lt;&gt; "",D62 = ""), "No P/N!","")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D40:E42"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="D25:E26"/>
+  <mergeCells count="2">
+    <mergeCell ref="A54:G54"/>
     <mergeCell ref="D17:E17"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
+  <conditionalFormatting sqref="I3:I223">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(I3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>